<commit_message>
remove unnecessary file tracking and tidy the archive summary read methods
</commit_message>
<xml_diff>
--- a/PREPARE-TIMES-NZ/data_raw/archive/TIMES-NZ/SysSettings.xlsx
+++ b/PREPARE-TIMES-NZ/data_raw/archive/TIMES-NZ/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greeda\git\TIMES-NZ-Model-Files\TIMES-NZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SearleL\Repos\TIMES-NZ-Model-Files\PREPARE-TIMES-NZ\data_raw\archive\TIMES-NZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E78621-0917-4637-9CE3-C11D9069C380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2144AFE-D059-4814-82B1-02FEF27BF658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="-18120" windowWidth="29040" windowHeight="17520" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="853" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="22" r:id="rId1"/>
@@ -11925,7 +11925,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="69" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="68" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -11957,6 +11956,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="69" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3853">
     <cellStyle name="20 % - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -16250,7 +16250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8D1A57-CDAE-4682-907E-2EE2CABFDB12}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -16315,7 +16315,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>153</v>
       </c>
     </row>
@@ -16409,8 +16409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:E24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16446,178 +16446,178 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="35" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="27">
+      <c r="B13" s="40">
         <v>1</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="40">
         <v>1</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="40">
         <v>1</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="27">
+      <c r="B14" s="40">
         <v>2</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="40">
         <v>2</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="40">
         <v>4</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="27">
+      <c r="B15" s="40">
         <v>5</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="40">
         <v>2</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="40">
         <v>5</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="27">
+      <c r="B16" s="40">
         <v>5</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="40">
         <v>3</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="40">
         <v>5</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="27">
+      <c r="B17" s="40">
         <v>5</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="40">
         <v>5</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="40">
         <v>5</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="27">
+      <c r="B18" s="40">
         <v>5</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="40">
         <v>5</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="40">
         <v>5</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="27">
+      <c r="B19" s="40">
         <v>5</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="40">
         <v>5</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="40">
         <v>5</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="27">
+      <c r="B20" s="40">
         <v>5</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="40">
         <v>5</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="40">
         <v>5</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="27">
+      <c r="B21" s="40">
         <v>5</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="40">
         <v>5</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="40">
         <v>5</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="27">
+      <c r="B22" s="40">
         <v>5</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="40">
         <v>5</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="40">
         <v>5</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="27">
+      <c r="B23" s="40">
         <v>5</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="40">
         <v>5</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27">
+      <c r="D23" s="40"/>
+      <c r="E23" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="27"/>
-      <c r="C24" s="27">
+      <c r="B24" s="40"/>
+      <c r="C24" s="40">
         <v>5</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27">
+      <c r="D24" s="40"/>
+      <c r="E24" s="40">
         <v>1</v>
       </c>
     </row>
@@ -16649,58 +16649,58 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="29">
         <v>0</v>
       </c>
     </row>
@@ -17204,26 +17204,26 @@
       <c r="K26" s="23"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
+      <c r="B27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
+      <c r="B28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
@@ -17806,14 +17806,14 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="14"/>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
     </row>
@@ -17835,7 +17835,7 @@
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="38" t="s">
         <v>95</v>
       </c>
       <c r="C39" s="13"/>
@@ -17861,7 +17861,7 @@
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="40"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="23"/>
       <c r="D40" s="23"/>
       <c r="E40" s="23"/>
@@ -17885,7 +17885,7 @@
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="40"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="23"/>
       <c r="D41" s="23"/>
       <c r="E41" s="23"/>
@@ -17909,7 +17909,7 @@
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="40"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="23"/>
       <c r="D42" s="23"/>
       <c r="E42" s="23"/>
@@ -17970,7 +17970,7 @@
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="38" t="s">
         <v>96</v>
       </c>
       <c r="C45" s="13"/>
@@ -17996,7 +17996,7 @@
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="40"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="23"/>
       <c r="D46" s="23"/>
       <c r="E46" s="23"/>
@@ -18067,7 +18067,7 @@
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="38" t="s">
         <v>97</v>
       </c>
       <c r="C49" s="13">
@@ -18103,7 +18103,7 @@
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B50" s="40"/>
+      <c r="B50" s="39"/>
       <c r="C50" s="13">
         <v>11</v>
       </c>
@@ -18137,7 +18137,7 @@
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="40"/>
+      <c r="B51" s="39"/>
       <c r="C51" s="13">
         <v>11</v>
       </c>
@@ -18171,7 +18171,7 @@
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="40"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="13">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Initial build for PREPARE-TIMES-NZ (#78)
This is the first version of a method for the proposed data_raw -> data_intermediate workflow in PREPARE-TIMES-NZ, and the user config files that define how data should sit in the generated excel files to be read by Veda. It contains documentation on the methods and structures, and the scripts in PREPARE-TIMES-NZ/scripts/stage_2_baseyear act as an initial template for how these might work for other components of TIMES-NZ in future. 

We note that there is a bit of tidying to do on this first pass.
</commit_message>
<xml_diff>
--- a/PREPARE-TIMES-NZ/data_raw/archive/TIMES-NZ/SysSettings.xlsx
+++ b/PREPARE-TIMES-NZ/data_raw/archive/TIMES-NZ/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greeda\git\TIMES-NZ-Model-Files\TIMES-NZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SearleL\Repos\TIMES-NZ-Model-Files\PREPARE-TIMES-NZ\data_raw\archive\TIMES-NZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E78621-0917-4637-9CE3-C11D9069C380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2144AFE-D059-4814-82B1-02FEF27BF658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5025" yWindow="-18120" windowWidth="29040" windowHeight="17520" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="853" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Documentation" sheetId="22" r:id="rId1"/>
@@ -11925,7 +11925,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="69" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="68" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -11957,6 +11956,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="69" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3853">
     <cellStyle name="20 % - Accent1" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -16250,7 +16250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8D1A57-CDAE-4682-907E-2EE2CABFDB12}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -16315,7 +16315,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>153</v>
       </c>
     </row>
@@ -16409,8 +16409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:E24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16446,178 +16446,178 @@
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="35" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="27">
+      <c r="B13" s="40">
         <v>1</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="40">
         <v>1</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="40">
         <v>1</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="27">
+      <c r="B14" s="40">
         <v>2</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="40">
         <v>2</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="40">
         <v>4</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="27">
+      <c r="B15" s="40">
         <v>5</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="40">
         <v>2</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="40">
         <v>5</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="27">
+      <c r="B16" s="40">
         <v>5</v>
       </c>
-      <c r="C16" s="27">
+      <c r="C16" s="40">
         <v>3</v>
       </c>
-      <c r="D16" s="27">
+      <c r="D16" s="40">
         <v>5</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="27">
+      <c r="B17" s="40">
         <v>5</v>
       </c>
-      <c r="C17" s="27">
+      <c r="C17" s="40">
         <v>5</v>
       </c>
-      <c r="D17" s="27">
+      <c r="D17" s="40">
         <v>5</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="27">
+      <c r="B18" s="40">
         <v>5</v>
       </c>
-      <c r="C18" s="27">
+      <c r="C18" s="40">
         <v>5</v>
       </c>
-      <c r="D18" s="27">
+      <c r="D18" s="40">
         <v>5</v>
       </c>
-      <c r="E18" s="27">
+      <c r="E18" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B19" s="27">
+      <c r="B19" s="40">
         <v>5</v>
       </c>
-      <c r="C19" s="27">
+      <c r="C19" s="40">
         <v>5</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="40">
         <v>5</v>
       </c>
-      <c r="E19" s="27">
+      <c r="E19" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B20" s="27">
+      <c r="B20" s="40">
         <v>5</v>
       </c>
-      <c r="C20" s="27">
+      <c r="C20" s="40">
         <v>5</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="40">
         <v>5</v>
       </c>
-      <c r="E20" s="27">
+      <c r="E20" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B21" s="27">
+      <c r="B21" s="40">
         <v>5</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="40">
         <v>5</v>
       </c>
-      <c r="D21" s="27">
+      <c r="D21" s="40">
         <v>5</v>
       </c>
-      <c r="E21" s="27">
+      <c r="E21" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B22" s="27">
+      <c r="B22" s="40">
         <v>5</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="40">
         <v>5</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="40">
         <v>5</v>
       </c>
-      <c r="E22" s="27">
+      <c r="E22" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B23" s="27">
+      <c r="B23" s="40">
         <v>5</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="40">
         <v>5</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27">
+      <c r="D23" s="40"/>
+      <c r="E23" s="40">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="27"/>
-      <c r="C24" s="27">
+      <c r="B24" s="40"/>
+      <c r="C24" s="40">
         <v>5</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27">
+      <c r="D24" s="40"/>
+      <c r="E24" s="40">
         <v>1</v>
       </c>
     </row>
@@ -16649,58 +16649,58 @@
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="30" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="29">
         <v>0</v>
       </c>
     </row>
@@ -17204,26 +17204,26 @@
       <c r="K26" s="23"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
+      <c r="B27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
     </row>
     <row r="28" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33"/>
+      <c r="B28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
     </row>
     <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
@@ -17806,14 +17806,14 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="14"/>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="D37" s="38"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
-      <c r="G37" s="38"/>
-      <c r="H37" s="38"/>
+      <c r="D37" s="37"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
     </row>
@@ -17835,7 +17835,7 @@
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B39" s="39" t="s">
+      <c r="B39" s="38" t="s">
         <v>95</v>
       </c>
       <c r="C39" s="13"/>
@@ -17861,7 +17861,7 @@
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B40" s="40"/>
+      <c r="B40" s="39"/>
       <c r="C40" s="23"/>
       <c r="D40" s="23"/>
       <c r="E40" s="23"/>
@@ -17885,7 +17885,7 @@
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B41" s="40"/>
+      <c r="B41" s="39"/>
       <c r="C41" s="23"/>
       <c r="D41" s="23"/>
       <c r="E41" s="23"/>
@@ -17909,7 +17909,7 @@
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B42" s="40"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="23"/>
       <c r="D42" s="23"/>
       <c r="E42" s="23"/>
@@ -17970,7 +17970,7 @@
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="39" t="s">
+      <c r="B45" s="38" t="s">
         <v>96</v>
       </c>
       <c r="C45" s="13"/>
@@ -17996,7 +17996,7 @@
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="40"/>
+      <c r="B46" s="39"/>
       <c r="C46" s="23"/>
       <c r="D46" s="23"/>
       <c r="E46" s="23"/>
@@ -18067,7 +18067,7 @@
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="39" t="s">
+      <c r="B49" s="38" t="s">
         <v>97</v>
       </c>
       <c r="C49" s="13">
@@ -18103,7 +18103,7 @@
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B50" s="40"/>
+      <c r="B50" s="39"/>
       <c r="C50" s="13">
         <v>11</v>
       </c>
@@ -18137,7 +18137,7 @@
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="40"/>
+      <c r="B51" s="39"/>
       <c r="C51" s="13">
         <v>11</v>
       </c>
@@ -18171,7 +18171,7 @@
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="40"/>
+      <c r="B52" s="39"/>
       <c r="C52" s="13">
         <v>11</v>
       </c>

</xml_diff>